<commit_message>
feat(DataMarketing-CustomerLead): update import excel
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/template-customer-lead.xlsx
+++ b/src/storage/app/excel-exporter/templates/template-customer-lead.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">Họ Và Tên</t>
   </si>
@@ -41,6 +41,24 @@
     <t xml:space="preserve">Nguồn tìm kiếm</t>
   </si>
   <si>
+    <t xml:space="preserve">Nguyễn Văn Đáng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20-09-1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0823573189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dangnguyenvan.info@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FANPAGE</t>
+  </si>
+  <si>
     <t xml:space="preserve">DATA_MKT</t>
   </si>
   <si>
@@ -51,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">là Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FANPAGE</t>
   </si>
   <si>
     <t xml:space="preserve">là Fanpage</t>
@@ -244,10 +259,10 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.49"/>
@@ -282,7 +297,24 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F2" s="5"/>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F3" s="5"/>
@@ -3285,6 +3317,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="dangnguyenvan.info@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3303,10 +3338,10 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A2:F2 A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.76"/>
@@ -3314,90 +3349,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>